<commit_message>
mer bilder och korrlängder
</commit_message>
<xml_diff>
--- a/Korrlängd, elfouhaily.xlsx
+++ b/Korrlängd, elfouhaily.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oskap\Documents\GitHub\Wavespectrum-to-Surface-2D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E77D7B75-29BD-4EA8-80A6-30246A1E57C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9BCD97-179F-4C61-8B03-855A6410A2FB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{B04EF0F6-0925-485F-90D6-A1F44EED2C62}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Correlation lengths, Elfouhaily surface 50mx50m</t>
   </si>
@@ -35,14 +35,28 @@
   <si>
     <t>Development(down):</t>
   </si>
+  <si>
+    <t>Calculated using l = std(rms(corrcoef(ZSURF)))</t>
+  </si>
+  <si>
+    <t>Calculated using l = rms(std(corrcoef(ZSURF)))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -58,12 +72,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,13 +85,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,81 +429,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65703398-0BF9-469D-A14B-7FCDF29CB2A4}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3">
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C4">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>0.84</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.52139999999999997</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>0.58909999999999996</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>0.57779999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="L5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0.84</v>
+      </c>
+      <c r="N5">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="O5" s="2">
+        <v>4.0645999999999998E-4</v>
+      </c>
+      <c r="P5" s="2">
+        <v>6.9902999999999998E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C6" s="6">
         <v>0.58620000000000005</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6">
+      <c r="D6">
+        <v>0.55389999999999995</v>
+      </c>
+      <c r="E6">
+        <v>0.61309999999999998</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2.4142E-4</v>
+      </c>
+      <c r="O6">
+        <v>4.3E-3</v>
+      </c>
+      <c r="P6">
+        <v>4.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="7">
         <v>0.57640000000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="D7">
+        <v>0.58160000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.63119999999999998</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7" s="5">
+        <v>4.6767999999999998E-6</v>
+      </c>
+      <c r="O7" s="2">
+        <v>3.6069999999999999E-4</v>
+      </c>
+      <c r="P7">
+        <v>5.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="7">
         <v>0.57640000000000002</v>
+      </c>
+      <c r="D8">
+        <v>0.56889999999999996</v>
+      </c>
+      <c r="E8">
+        <v>0.55369999999999997</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8" s="4">
+        <v>3.6619999999999998E-6</v>
+      </c>
+      <c r="O8" s="2">
+        <v>9.1111000000000002E-5</v>
+      </c>
+      <c r="P8" s="3">
+        <v>4.1000000000000003E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>